<commit_message>
addition of xml related queries
</commit_message>
<xml_diff>
--- a/Db design.xlsx
+++ b/Db design.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="108" windowWidth="8580" windowHeight="7968"/>
+    <workbookView xWindow="480" yWindow="108" windowWidth="8580" windowHeight="7968" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="rateRule" sheetId="1" r:id="rId1"/>
-    <sheet name="userRateConditioning" sheetId="2" r:id="rId2"/>
-    <sheet name="userRateConditionRefrenceLink" sheetId="10" r:id="rId3"/>
-    <sheet name="rateConditioningUserDevicesLink" sheetId="9" r:id="rId4"/>
-    <sheet name="rateConditionUserCountryLink" sheetId="8" r:id="rId5"/>
-    <sheet name="rateConditionLanguageLink" sheetId="7" r:id="rId6"/>
-    <sheet name="RateConditioningMembershipLink" sheetId="11" r:id="rId7"/>
-    <sheet name="RateInEligiblity" sheetId="4" r:id="rId8"/>
-    <sheet name="rateModification" sheetId="5" r:id="rId9"/>
-    <sheet name="rateRuleConditioningLink" sheetId="6" r:id="rId10"/>
+    <sheet name="rate_rule" sheetId="1" r:id="rId1"/>
+    <sheet name="user_rate_condition" sheetId="2" r:id="rId2"/>
+    <sheet name="rate_condition_refrence_link" sheetId="10" r:id="rId3"/>
+    <sheet name="rate_condition_user_device_link" sheetId="9" r:id="rId4"/>
+    <sheet name="user_condition_user_contry_link" sheetId="8" r:id="rId5"/>
+    <sheet name="rate_condition_language_link" sheetId="7" r:id="rId6"/>
+    <sheet name="rate_condition_membership_link" sheetId="11" r:id="rId7"/>
+    <sheet name="user_rate_ineligiblity" sheetId="4" r:id="rId8"/>
+    <sheet name="rate_modification" sheetId="5" r:id="rId9"/>
+    <sheet name="rate_rule_condition_link" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="57">
   <si>
     <t>description</t>
   </si>
@@ -154,21 +154,6 @@
     <t>user_rate_condition_id</t>
   </si>
   <si>
-    <t>pg001</t>
-  </si>
-  <si>
-    <t>pg004</t>
-  </si>
-  <si>
-    <t>pg007</t>
-  </si>
-  <si>
-    <t>pg009</t>
-  </si>
-  <si>
-    <t>pg0010</t>
-  </si>
-  <si>
     <t>always_eligible_membership_id</t>
   </si>
   <si>
@@ -200,6 +185,15 @@
   </si>
   <si>
     <t>rate_ineligblity_id</t>
+  </si>
+  <si>
+    <t>pg002</t>
+  </si>
+  <si>
+    <t>pg006</t>
+  </si>
+  <si>
+    <t>pg0020</t>
   </si>
 </sst>
 </file>
@@ -247,7 +241,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -255,17 +249,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -585,7 +603,7 @@
         <v>34</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>36</v>
@@ -633,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,104 +716,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="50.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>57</v>
+      <c r="D1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="8">
         <v>15</v>
       </c>
-      <c r="E2" t="b">
+      <c r="E2" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F2" t="b">
+      <c r="F2" s="8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="8">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -804,10 +821,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,10 +835,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -830,14 +847,6 @@
       </c>
       <c r="B2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -850,7 +859,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -864,7 +873,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -909,12 +918,12 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -923,7 +932,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -976,7 +985,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,7 +999,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1036,7 +1045,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,7 +1059,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1058,7 +1067,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1066,7 +1075,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1074,7 +1083,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1082,7 +1091,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1090,7 +1099,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>